<commit_message>
fully functional configurable dashboard
</commit_message>
<xml_diff>
--- a/R/practice/configure shiny ui/bbos_developer_config.xlsx
+++ b/R/practice/configure shiny ui/bbos_developer_config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Catherine\Documents\git repos\operating-system\development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Catherine\Documents\Development\learning\R\practice\configure shiny ui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE60558F-79F9-41E6-9225-FCD023C14C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279009F7-2DCD-4B4E-9149-C11C1BD88D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AAD3DC31-2CEF-44B9-956F-90112AADF1F0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
   <si>
     <t>module</t>
   </si>
@@ -145,6 +145,30 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>home1</t>
+  </si>
+  <si>
+    <t>data1</t>
+  </si>
+  <si>
+    <t>nesting1</t>
+  </si>
+  <si>
+    <t>rois1</t>
+  </si>
+  <si>
+    <t>reoptimise1</t>
+  </si>
+  <si>
+    <t>download1</t>
+  </si>
+  <si>
+    <t>modellingtool1</t>
+  </si>
+  <si>
+    <t>modellingtool</t>
   </si>
 </sst>
 </file>
@@ -499,7 +523,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -508,6 +532,7 @@
     <col min="2" max="2" width="13.26953125" customWidth="1"/>
     <col min="3" max="3" width="23.81640625" customWidth="1"/>
     <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="6" max="6" width="22.54296875" customWidth="1"/>
     <col min="7" max="7" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -565,9 +590,8 @@
       <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="str">
-        <f>_xlfn.CONCAT(F2,1)</f>
-        <v>home1</v>
+      <c r="I2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -595,9 +619,8 @@
       <c r="H3" t="s">
         <v>7</v>
       </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I8" si="0">_xlfn.CONCAT(F3,1)</f>
-        <v>data1</v>
+      <c r="I3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -617,7 +640,7 @@
         <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
@@ -625,9 +648,8 @@
       <c r="H4" t="s">
         <v>7</v>
       </c>
-      <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>modelling tool1</v>
+      <c r="I4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -655,9 +677,8 @@
       <c r="H5" t="s">
         <v>7</v>
       </c>
-      <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>nesting1</v>
+      <c r="I5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -685,9 +706,8 @@
       <c r="H6" t="s">
         <v>7</v>
       </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>rois1</v>
+      <c r="I6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -715,9 +735,8 @@
       <c r="H7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>reoptimise1</v>
+      <c r="I7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -745,9 +764,8 @@
       <c r="H8" t="s">
         <v>7</v>
       </c>
-      <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>download1</v>
+      <c r="I8" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>